<commit_message>
finished the grasp time and end for SNS, now working on the deposit time and end
</commit_message>
<xml_diff>
--- a/datalogs/Data Analysis/August17th_Analysis.xlsx
+++ b/datalogs/Data Analysis/August17th_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravesh\Desktop\Research\FRR\FRR Software Interface\FRR-Software-Interface\datalogs\Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF713F34-7F2E-4F91-BFEF-A59179E8C759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593FB4D-8270-41EC-B6D6-554B939A6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{45D17099-BCB3-43AF-8462-D5158977141E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{45D17099-BCB3-43AF-8462-D5158977141E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{261EAD39-7684-4EC3-BEB4-AE778078DB6B}">
+    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{261EAD39-7684-4EC3-BEB4-AE778078DB6B}">
       <text>
         <r>
           <rPr>
@@ -223,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{68AE7661-017B-4190-B90E-88498E8B01C6}">
+    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{68AE7661-017B-4190-B90E-88498E8B01C6}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{973EBAC5-49E9-4425-9BFC-3FCFB7D74CAF}">
+    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{973EBAC5-49E9-4425-9BFC-3FCFB7D74CAF}">
       <text>
         <r>
           <rPr>
@@ -274,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{BEAD9D9B-B4F3-4205-AE90-B7F3C6C849C2}">
+    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{BEAD9D9B-B4F3-4205-AE90-B7F3C6C849C2}">
       <text>
         <r>
           <rPr>
@@ -298,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{5EB0F785-3688-46C8-A6D6-143450018931}">
+    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{5EB0F785-3688-46C8-A6D6-143450018931}">
       <text>
         <r>
           <rPr>
@@ -323,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{FF71CBEB-4499-468A-A294-8FD80859A6B2}">
+    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{FF71CBEB-4499-468A-A294-8FD80859A6B2}">
       <text>
         <r>
           <rPr>
@@ -348,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{54B32650-2908-4A23-87E9-FF6084CAAA15}">
+    <comment ref="W1" authorId="1" shapeId="0" xr:uid="{54B32650-2908-4A23-87E9-FF6084CAAA15}">
       <text>
         <r>
           <rPr>
@@ -373,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{56A4EC55-9BD7-414C-B93E-6231ACC2F000}">
+    <comment ref="X1" authorId="1" shapeId="0" xr:uid="{56A4EC55-9BD7-414C-B93E-6231ACC2F000}">
       <text>
         <r>
           <rPr>
@@ -400,12 +400,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q24" authorId="1" shapeId="0" xr:uid="{E218CC52-6CB3-40BE-A39E-798AF6903E23}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ravesh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+no ZR, just SR
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="129">
   <si>
     <t>User</t>
   </si>
@@ -651,6 +676,147 @@
   </si>
   <si>
     <t>2023-08-17 11:05:06,358</t>
+  </si>
+  <si>
+    <t>In progress Start time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:03:48,035</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:03:16,214</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:03:08,840</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:03:59,707</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:04:16,410</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:04:19,354</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:05:07,357</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:06:43,250</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:07:30,309</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:08:17,532</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:08:29,396</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:08:56,467</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:08:57,869</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:09:33,937</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:10:24,891</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:11:05,743</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:11:49,802</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:12:41,951</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:13:22,843</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:14:05,846</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:14:17,379</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:19:02,617</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:20:09,557</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:20:29,408</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:20:31,160</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:21:28,813</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:21:44,204</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:22:01,780</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:22:53,705</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:23:35,199</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:24:33,268</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:25:14,613</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:25:32,865</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:27:02,611</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:27:55,897</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:28:21,397</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:29:02,395</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:29:16,862</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:30:26,733</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:30:44,276</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:31:46,125</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:32:14,482</t>
+  </si>
+  <si>
+    <t>2023-08-17 11:33:41,827</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>8/17/2023  11:06:40 AM , 862</t>
   </si>
 </sst>
 </file>
@@ -1061,13 +1227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F998FF6-62B6-43DC-AAC1-081D9B2F4963}">
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:AA89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="O24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="P24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V33" sqref="V33"/>
+      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,16 +1248,17 @@
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="14" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" customWidth="1"/>
+    <col min="15" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="14" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,39 +1301,45 @@
       <c r="N1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1180,7 +1353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1195,7 +1368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1210,7 +1383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1225,7 +1398,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1240,7 +1413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1255,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1270,7 +1443,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1285,7 +1458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1300,7 +1473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1315,7 +1488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1330,7 +1503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1344,7 +1517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1359,7 +1532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1374,7 +1547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1389,7 +1562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1404,7 +1577,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1419,7 +1592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1434,7 +1607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1449,7 +1622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1464,7 +1637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1479,7 +1652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1494,7 +1667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1526,23 +1699,29 @@
       <c r="N24" t="s">
         <v>76</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>69</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <v>-20</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <v>37</v>
       </c>
-      <c r="X24">
+      <c r="Z24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1563,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I34" si="2">H25+1</f>
+        <f t="shared" ref="I25:I46" si="2">H25+1</f>
         <v>3</v>
       </c>
       <c r="J25" t="s">
@@ -1575,23 +1754,29 @@
       <c r="N25" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="O25" t="s">
+        <v>84</v>
+      </c>
+      <c r="P25" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>72</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <v>-177</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <v>-139</v>
       </c>
-      <c r="X25">
+      <c r="Z25">
         <v>-103.2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1627,23 +1812,29 @@
       <c r="N26" t="s">
         <v>76</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="O26" t="s">
+        <v>88</v>
+      </c>
+      <c r="P26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>74</v>
       </c>
-      <c r="V26">
+      <c r="X26">
         <v>-181</v>
       </c>
-      <c r="W26">
+      <c r="Y26">
         <v>-160</v>
       </c>
-      <c r="X26">
+      <c r="Z26">
         <v>-103.01</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1673,29 +1864,35 @@
       <c r="L27" t="s">
         <v>67</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="O27" t="s">
+        <v>90</v>
+      </c>
+      <c r="P27" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>77</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="S27" t="s">
         <v>78</v>
       </c>
-      <c r="R27" t="s">
+      <c r="T27" t="s">
         <v>79</v>
       </c>
-      <c r="V27">
+      <c r="X27">
         <v>-15</v>
       </c>
-      <c r="W27">
+      <c r="Y27">
         <v>183</v>
       </c>
-      <c r="X27">
+      <c r="Z27">
         <v>-102.76</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1725,8 +1922,17 @@
       <c r="L28" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1756,8 +1962,14 @@
       <c r="L29" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>93</v>
+      </c>
+      <c r="P29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1790,8 +2002,14 @@
       <c r="L30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>95</v>
+      </c>
+      <c r="P30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1821,8 +2039,14 @@
       <c r="L31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>97</v>
+      </c>
+      <c r="P31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1852,8 +2076,14 @@
       <c r="L32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>99</v>
+      </c>
+      <c r="P32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1883,8 +2113,14 @@
       <c r="L33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>101</v>
+      </c>
+      <c r="P33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1914,8 +2150,14 @@
       <c r="L34" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>103</v>
+      </c>
+      <c r="P34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1931,8 +2173,27 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J35" t="s">
+        <v>63</v>
+      </c>
+      <c r="L35" t="s">
+        <v>66</v>
+      </c>
+      <c r="O35" t="s">
+        <v>105</v>
+      </c>
+      <c r="P35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1949,8 +2210,27 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J36" t="s">
+        <v>63</v>
+      </c>
+      <c r="L36" t="s">
+        <v>67</v>
+      </c>
+      <c r="O36" t="s">
+        <v>107</v>
+      </c>
+      <c r="P36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1967,8 +2247,27 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>61</v>
+      </c>
+      <c r="L37" t="s">
+        <v>127</v>
+      </c>
+      <c r="O37" t="s">
+        <v>109</v>
+      </c>
+      <c r="P37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1985,8 +2284,27 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>61</v>
+      </c>
+      <c r="L38" t="s">
+        <v>67</v>
+      </c>
+      <c r="O38" t="s">
+        <v>111</v>
+      </c>
+      <c r="P38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2003,8 +2321,27 @@
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+      <c r="L39" t="s">
+        <v>67</v>
+      </c>
+      <c r="O39" t="s">
+        <v>113</v>
+      </c>
+      <c r="P39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2021,8 +2358,27 @@
       <c r="F40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J40" t="s">
+        <v>61</v>
+      </c>
+      <c r="L40" t="s">
+        <v>127</v>
+      </c>
+      <c r="O40" t="s">
+        <v>115</v>
+      </c>
+      <c r="P40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2039,8 +2395,27 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>62</v>
+      </c>
+      <c r="L41" t="s">
+        <v>67</v>
+      </c>
+      <c r="O41" t="s">
+        <v>117</v>
+      </c>
+      <c r="P41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2057,8 +2432,27 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>63</v>
+      </c>
+      <c r="L42" t="s">
+        <v>66</v>
+      </c>
+      <c r="O42" t="s">
+        <v>119</v>
+      </c>
+      <c r="P42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -2075,8 +2469,27 @@
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J43" t="s">
+        <v>63</v>
+      </c>
+      <c r="L43" t="s">
+        <v>66</v>
+      </c>
+      <c r="O43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -2093,8 +2506,27 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J44" t="s">
+        <v>63</v>
+      </c>
+      <c r="L44" t="s">
+        <v>67</v>
+      </c>
+      <c r="O44" t="s">
+        <v>123</v>
+      </c>
+      <c r="P44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2111,8 +2543,27 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" t="s">
+        <v>67</v>
+      </c>
+      <c r="O45" t="s">
+        <v>125</v>
+      </c>
+      <c r="P45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2126,7 +2577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2141,7 +2592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2780,7 +3231,7 @@
   <dimension ref="A2:AG16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>